<commit_message>
Traffic light system with pedestrian light code
</commit_message>
<xml_diff>
--- a/Team Exemplary.xlsx
+++ b/Team Exemplary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nurus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHMED\Documents\GitHub\Micro-Controller-group-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511C7202-AC69-4341-8958-51E1079A87DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3025E286-A456-4E8B-B96A-F48DCF2A5A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Team Exemplary</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Siddiquy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neaz </t>
+  </si>
+  <si>
+    <t>Mahmud</t>
   </si>
 </sst>
 </file>
@@ -363,25 +369,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="24.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.90625" customWidth="1"/>
+    <col min="3" max="3" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -389,7 +395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -397,12 +403,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>